<commit_message>
Added Enums,updated config,Reports classes
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata.xlsx
+++ b/src/test/resources/Testdata.xlsx
@@ -8,15 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -24,19 +23,34 @@
     <t>password</t>
   </si>
   <si>
-    <t>loginTest</t>
-  </si>
-  <si>
-    <t>Admin123</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
     <t>prabhu</t>
   </si>
   <si>
+    <t>tileValidationTest</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>expectedTitle</t>
+  </si>
+  <si>
+    <t>OrangeHRM</t>
+  </si>
+  <si>
     <t>testcaseName</t>
+  </si>
+  <si>
+    <t>runTestcase</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -368,22 +382,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -391,27 +407,45 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -429,16 +463,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>